<commit_message>
feat: add string to the end of the cell
</commit_message>
<xml_diff>
--- a/modelo.xlsx
+++ b/modelo.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Documents\Development\Java\Apache Poi\escrever-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A45716A-AC87-4B53-9766-99C27400DCB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D635E385-A1A5-46AE-AF0D-D202AAA0ADA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="16440" xr2:uid="{4B696E45-CD18-43E0-B4C1-33F4C8289159}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,22 +36,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>a1</t>
   </si>
   <si>
     <t>a2</t>
   </si>
-  <si>
-    <t>Novo Valor</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -404,6 +400,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="53.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -412,7 +411,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>